<commit_message>
implemented my own wait method
</commit_message>
<xml_diff>
--- a/mavenHybrid/webdriver/excelLib.xlsx
+++ b/mavenHybrid/webdriver/excelLib.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6390" windowWidth="15420" xWindow="0" yWindow="2445"/>
+    <workbookView activeTab="1" windowHeight="6390" windowWidth="15060" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
     <sheet name="login" r:id="rId1" sheetId="1"/>
@@ -13,11 +13,12 @@
     <sheet name="dragDrop" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="40">
   <si>
     <t>SpecialActionType</t>
   </si>
@@ -112,35 +113,31 @@
     <t>NO</t>
   </si>
   <si>
-    <t>file:///E:/webs/hero/the-internet.herokuapp.com/drag_and_drop.html</t>
-  </si>
-  <si>
-    <t>drag drop by element</t>
-  </si>
-  <si>
     <t>close</t>
   </si>
   <si>
     <t>dragDrop</t>
   </si>
   <si>
+    <t>debug</t>
+  </si>
+  <si>
     <t>SKIPPED</t>
   </si>
   <si>
-    <t>FAIL no such element: Unable to locate element: {"method":"id","selector":"logoutLink"}
-  (Session info: chrome=56.0.2924.87)
-  (Driver info: chromedriver=2.28.455520 (cc17746adff54984afff480136733114c6b3704b),platform=Windows NT 6.3.9600 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 235 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: 'b526bd5', time: '2017-03-07 11:11:07 -0800'
-System info: host: 'sai', ip: '127.0.0.1', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '1.8.0_121'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.28.455520 (cc17746adff54984afff480136733114c6b3704b), userDataDir=C:\Users\partha\AppData\Local\Temp\scoped_dir10600_12355}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=WIN8_1, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=}]
-Session ID: 181cbdd54aced2cca9ce64f8d82ad5ee
-*** Element info: {Using=id, value=logoutLink}</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>drag drop by coordinates</t>
+  </si>
+  <si>
+    <t>file:///E:/webs/jquiryUI/jqueryui.com/draggable/index.html</t>
+  </si>
+  <si>
+    <t>FAIL null</t>
+  </si>
+  <si>
+    <t>switchtoframe</t>
+  </si>
+  <si>
+    <t>Phantom JS</t>
   </si>
 </sst>
 </file>
@@ -654,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -716,10 +713,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3">
@@ -733,7 +727,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4">
@@ -750,7 +744,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5">
@@ -767,7 +761,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6">
@@ -781,7 +775,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7">
@@ -794,8 +788,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="C8" t="s">
+    <row customFormat="1" r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -805,14 +802,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="C9" t="s">
+    <row customFormat="1" r="9" spans="1:10">
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D9">
         <v>5000</v>
       </c>
       <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="10" spans="1:10">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" spans="1:10">
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="12" spans="1:10">
+      <c r="G12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -834,7 +849,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C8 C2 C4 B3:B7" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C7 B8" type="list">
       <formula1>"geturl,find element"</formula1>
     </dataValidation>
   </dataValidations>
@@ -847,7 +862,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -881,13 +896,13 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -901,21 +916,21 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1139,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1156,7 +1171,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1179,53 +1194,70 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row customFormat="1" r="2" spans="1:8">
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="3" spans="1:8">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="4" spans="1:8">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>147</v>
+      </c>
+      <c r="F4">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row customFormat="1" r="5" spans="1:8">
+      <c r="C5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customFormat="1" r="6" spans="1:8">
+      <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="C4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4">
-        <v>5000</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list">
       <formula1>"geturl,find element"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Implemented my own wait method Removed unwanted codes,supports nested level sheet execution upto any level
</commit_message>
<xml_diff>
--- a/mavenHybrid/webdriver/excelLib.xlsx
+++ b/mavenHybrid/webdriver/excelLib.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6390" windowWidth="15060" xWindow="0" yWindow="2445"/>
+    <workbookView activeTab="3" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="3375"/>
   </bookViews>
   <sheets>
     <sheet name="login" r:id="rId1" sheetId="1"/>
     <sheet name="suite" r:id="rId2" sheetId="2"/>
     <sheet name="specialchar" r:id="rId3" sheetId="3"/>
     <sheet name="dragDrop" r:id="rId4" sheetId="4"/>
+    <sheet name="a" r:id="rId5" sheetId="5"/>
+    <sheet name="b" r:id="rId6" sheetId="6"/>
+    <sheet name="Sheet1" r:id="rId7" sheetId="7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
   <si>
     <t>SpecialActionType</t>
   </si>
@@ -98,46 +100,40 @@
     <t>specialchar</t>
   </si>
   <si>
-    <t>checkalllinks</t>
-  </si>
-  <si>
-    <t>checkallimages</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
+    <t>dragDrop</t>
+  </si>
+  <si>
+    <t>drag drop by coordinates</t>
+  </si>
+  <si>
+    <t>file:///E:/webs/jquiryUI/jqueryui.com/draggable/index.html</t>
+  </si>
+  <si>
+    <t>switchtoframe</t>
+  </si>
+  <si>
+    <t>FireFox</t>
+  </si>
+  <si>
+    <t>executesheet</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
+  </si>
+  <si>
     <t>sleep</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>dragDrop</t>
-  </si>
-  <si>
-    <t>debug</t>
-  </si>
-  <si>
-    <t>SKIPPED</t>
-  </si>
-  <si>
-    <t>drag drop by coordinates</t>
-  </si>
-  <si>
-    <t>file:///E:/webs/jquiryUI/jqueryui.com/draggable/index.html</t>
-  </si>
-  <si>
-    <t>FAIL null</t>
-  </si>
-  <si>
-    <t>switchtoframe</t>
-  </si>
-  <si>
-    <t>Phantom JS</t>
   </si>
 </sst>
 </file>
@@ -145,7 +141,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,24 +150,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -221,38 +202,80 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+  <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -651,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -788,7 +811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row customFormat="1" r="8" spans="1:10">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -802,54 +825,36 @@
         <v>12</v>
       </c>
     </row>
-    <row customFormat="1" r="9" spans="1:10">
-      <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9">
-        <v>5000</v>
+    <row r="9" spans="1:10">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customFormat="1" r="10" spans="1:10">
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customFormat="1" r="11" spans="1:10">
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customFormat="1" r="12" spans="1:10">
-      <c r="G12" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J1">
-    <cfRule dxfId="14" priority="1" stopIfTrue="1" type="expression">
+    <cfRule dxfId="20" priority="1" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
     </cfRule>
-    <cfRule dxfId="13" priority="2" stopIfTrue="1" type="expression">
+    <cfRule dxfId="19" priority="2" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule dxfId="12" priority="3" stopIfTrue="1" type="expression">
+    <cfRule dxfId="18" priority="3" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",H1)))</formula>
     </cfRule>
-    <cfRule dxfId="11" priority="4" stopIfTrue="1" type="expression">
+    <cfRule dxfId="17" priority="4" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C7 B8" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C7 B8:B9" type="list">
       <formula1>"geturl,find element"</formula1>
     </dataValidation>
   </dataValidations>
@@ -859,10 +864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -896,13 +901,13 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -910,54 +915,68 @@
         <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule dxfId="10" operator="equal" priority="1" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="16" operator="equal" priority="1" stopIfTrue="1" type="cellIs">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="9" operator="equal" priority="2" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="15" operator="equal" priority="2" stopIfTrue="1" type="cellIs">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule dxfId="8" operator="equal" priority="3" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="14" operator="equal" priority="3" stopIfTrue="1" type="cellIs">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="7" operator="equal" priority="4" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="13" operator="equal" priority="4" stopIfTrue="1" type="cellIs">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule dxfId="6" operator="equal" priority="5" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="12" operator="equal" priority="5" stopIfTrue="1" type="cellIs">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B4" type="list">
+    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B5" type="list">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C4" type="list">
+    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C5" type="list">
       <formula1>"FireFox,Chrome,Internet Explorer,Phantom JS"</formula1>
     </dataValidation>
   </dataValidations>
@@ -968,10 +987,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1026,124 +1045,42 @@
     </row>
     <row r="3" spans="1:9">
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="G9" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1">
-    <cfRule dxfId="5" priority="3" stopIfTrue="1" type="expression">
+    <cfRule dxfId="11" priority="3" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
     </cfRule>
-    <cfRule dxfId="4" priority="4" stopIfTrue="1" type="expression">
+    <cfRule dxfId="10" priority="4" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule dxfId="3" priority="5" stopIfTrue="1" type="expression">
+    <cfRule dxfId="9" priority="5" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",H1)))</formula>
     </cfRule>
-    <cfRule dxfId="2" priority="6" stopIfTrue="1" type="expression">
+    <cfRule dxfId="8" priority="6" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule dxfId="1" operator="containsText" priority="1" text="fail" type="containsText">
+    <cfRule dxfId="7" operator="containsText" priority="1" text="fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("fail",G1)))</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="containsText" priority="2" text="pass" type="containsText">
+    <cfRule dxfId="6" operator="containsText" priority="2" text="pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("pass",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C5" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list">
       <formula1>"geturl,find element"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1154,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1171,7 +1108,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1194,20 +1131,20 @@
         <v>5</v>
       </c>
     </row>
-    <row customFormat="1" r="2" spans="1:8">
+    <row r="2" spans="1:7">
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row customFormat="1" r="3" spans="1:8">
+    <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1216,42 +1153,31 @@
         <v>12</v>
       </c>
     </row>
-    <row customFormat="1" r="4" spans="1:8">
+    <row r="4" spans="1:7">
       <c r="C4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4">
+        <v>3000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
         <v>13</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>147</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>47</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row customFormat="1" r="5" spans="1:8">
-      <c r="C5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>5000</v>
-      </c>
       <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customFormat="1" r="6" spans="1:8">
-      <c r="C6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1263,4 +1189,267 @@
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I1">
+    <cfRule dxfId="5" priority="3" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
+    </cfRule>
+    <cfRule dxfId="4" priority="4" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule dxfId="3" priority="5" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("fail",H1)))</formula>
+    </cfRule>
+    <cfRule dxfId="2" priority="6" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("pass",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G3">
+    <cfRule dxfId="1" operator="containsText" priority="1" text="fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("fail",G1)))</formula>
+    </cfRule>
+    <cfRule dxfId="0" operator="containsText" priority="2" text="pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("pass",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C4" type="list">
+      <formula1>"geturl,find element"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C7" type="list">
+      <formula1>"geturl,find element"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fluent wait,update property files,dynamic xpath
</commit_message>
<xml_diff>
--- a/mavenHybrid/webdriver/excelLib.xlsx
+++ b/mavenHybrid/webdriver/excelLib.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="7" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="4050"/>
+    <workbookView activeTab="2" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="4050"/>
   </bookViews>
   <sheets>
     <sheet name="login" r:id="rId1" sheetId="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="55">
   <si>
     <t>SpecialActionType</t>
   </si>
@@ -128,40 +128,64 @@
     <t>NO</t>
   </si>
   <si>
-    <t>sendkeysappendname</t>
-  </si>
-  <si>
     <t>SKIPPED</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>sikuli</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/partha/Desktop/iframe.html</t>
+  </si>
+  <si>
+    <t>stdrightclick</t>
+  </si>
+  <si>
+    <t>for@@test</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>dupe</t>
+  </si>
+  <si>
+    <t>for@@new</t>
+  </si>
+  <si>
     <t>WARNING : sendkeys cell is blank,we sent current time value for this</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Sheet1</t>
-  </si>
-  <si>
-    <t>assertelement</t>
-  </si>
-  <si>
-    <t>FAIL java.lang.NullPointerException</t>
-  </si>
-  <si>
-    <t>sikuli</t>
-  </si>
-  <si>
-    <t>file:///C:/Users/partha/Desktop/iframe.html</t>
-  </si>
-  <si>
-    <t>stdrightclick</t>
+    <t>addtextwithtimestore</t>
+  </si>
+  <si>
+    <t>WARNING : store value(column 9) cell is blank,we sent current time value for this</t>
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>asserttitle</t>
+  </si>
+  <si>
+    <t>actiTIME - Login</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>FAIL,actual title is actiTIME - Login</t>
+  </si>
+  <si>
+    <t>www.gmail.com</t>
   </si>
 </sst>
 </file>
@@ -169,7 +193,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +207,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -230,12 +262,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -247,8 +282,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="19">
@@ -835,6 +874,9 @@
       <c r="G8" t="s">
         <v>12</v>
       </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J1">
@@ -865,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -908,7 +950,7 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -916,13 +958,13 @@
         <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -936,12 +978,12 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>34</v>
@@ -950,15 +992,15 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
         <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>34</v>
@@ -967,21 +1009,35 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -997,10 +1053,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B7" type="list">
+    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B8" type="list">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C7" type="list">
+    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C8" type="list">
       <formula1>"FireFox,Chrome,Internet Explorer,Phantom JS"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1011,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1022,9 +1078,9 @@
     <col min="1" max="1" customWidth="true" width="13.7109375" collapsed="true"/>
     <col min="2" max="3" customWidth="true" width="13.5703125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="25.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="46.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
@@ -1070,13 +1126,27 @@
     </row>
     <row r="3" spans="1:9">
       <c r="C3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1105,10 +1175,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2 C4" type="list">
       <formula1>"geturl,find element"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D4"/>
+  </hyperlinks>
   <pageMargins bottom="1" footer="0.51180555555555596" header="0.51180555555555596" left="0.75" right="0.75" top="1"/>
   <pageSetup copies="0" horizontalDpi="0" orientation="portrait" paperSize="0" verticalDpi="0"/>
 </worksheet>
@@ -1339,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1353,7 +1426,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="63.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1414,11 +1487,8 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1429,15 +1499,13 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="G6" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1453,14 +1521,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
@@ -1468,7 +1537,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1497,6 +1569,14 @@
       </c>
       <c r="G3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1513,7 +1593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1529,7 +1609,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1537,7 +1617,7 @@
     </row>
     <row r="3" spans="3:7">
       <c r="C3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>12</v>

</xml_diff>

<commit_message>
Added few Sikuli keywords
</commit_message>
<xml_diff>
--- a/mavenHybrid/webdriver/excelLib.xlsx
+++ b/mavenHybrid/webdriver/excelLib.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="4050"/>
+    <workbookView activeTab="9" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="4050"/>
   </bookViews>
   <sheets>
     <sheet name="login" r:id="rId1" sheetId="1"/>
@@ -15,13 +15,15 @@
     <sheet name="b" r:id="rId6" sheetId="6"/>
     <sheet name="Sheet1" r:id="rId7" sheetId="7"/>
     <sheet name="sikuli" r:id="rId8" sheetId="8"/>
+    <sheet name="sikuliselenium" r:id="rId9" sheetId="9"/>
+    <sheet name="seleniumupload" r:id="rId10" sheetId="10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="66">
   <si>
     <t>SpecialActionType</t>
   </si>
@@ -143,12 +145,6 @@
     <t>sikuli</t>
   </si>
   <si>
-    <t>file:///C:/Users/partha/Desktop/iframe.html</t>
-  </si>
-  <si>
-    <t>stdrightclick</t>
-  </si>
-  <si>
     <t>for@@test</t>
   </si>
   <si>
@@ -186,6 +182,69 @@
   </si>
   <si>
     <t>www.gmail.com</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/partha/Desktop/uploadfile.html</t>
+  </si>
+  <si>
+    <t>stdclick</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>paste</t>
+  </si>
+  <si>
+    <t>stdtype</t>
+  </si>
+  <si>
+    <t>clickenter</t>
+  </si>
+  <si>
+    <t>sikuliselenium</t>
+  </si>
+  <si>
+    <t>stddoubleclick</t>
+  </si>
+  <si>
+    <t>seleniumupload</t>
+  </si>
+  <si>
+    <t>FAIL unknown error: path is not absolute: file:///c:/users/partha/desktop/uploadfile.html
+  (Session info: chrome=56.0.2924.87)
+  (Driver info: chromedriver=2.28.455520 (cc17746adff54984afff480136733114c6b3704b),platform=Windows NT 6.3.9600 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 75 milliseconds
+Build info: version: 'unknown', revision: 'b526bd5', time: '2017-03-07 11:11:07 -0800'
+System info: host: 'SAI', ip: '127.0.0.1', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '1.8.0_121'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.28.455520 (cc17746adff54984afff480136733114c6b3704b), userDataDir=C:\Users\partha\AppData\Local\Temp\scoped_dir6436_12744}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=WIN8_1, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=accept}]
+Session ID: 5226fb890b8e5d324e74d64b9c653781</t>
+  </si>
+  <si>
+    <t>/log4j.properties</t>
+  </si>
+  <si>
+    <t>FAIL unknown error: path is not absolute: /log4j.properties
+  (Session info: chrome=56.0.2924.87)
+  (Driver info: chromedriver=2.28.455520 (cc17746adff54984afff480136733114c6b3704b),platform=Windows NT 6.3.9600 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 78 milliseconds
+Build info: version: 'unknown', revision: 'b526bd5', time: '2017-03-07 11:11:07 -0800'
+System info: host: 'SAI', ip: '127.0.0.1', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '1.8.0_121'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.28.455520 (cc17746adff54984afff480136733114c6b3704b), userDataDir=C:\Users\partha\AppData\Local\Temp\scoped_dir5260_12812}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=WIN8_1, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=accept}]
+Session ID: 4bd76188c6e65184753f8e2a304a92e0</t>
+  </si>
+  <si>
+    <t>FAIL unknown error: path is not absolute: /log4j.properties
+  (Session info: chrome=56.0.2924.87)
+  (Driver info: chromedriver=2.28.455520 (cc17746adff54984afff480136733114c6b3704b),platform=Windows NT 6.3.9600 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 78 milliseconds
+Build info: version: 'unknown', revision: 'b526bd5', time: '2017-03-07 11:11:07 -0800'
+System info: host: 'SAI', ip: '127.0.0.1', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '1.8.0_121'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.28.455520 (cc17746adff54984afff480136733114c6b3704b), userDataDir=C:\Users\partha\AppData\Local\Temp\scoped_dir6928_1117}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=WIN8_1, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=accept}]
+Session ID: ed86483c450b6d3ac31d332b40c59007</t>
   </si>
 </sst>
 </file>
@@ -193,12 +252,26 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -266,23 +339,29 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -730,7 +809,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -875,7 +954,7 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -905,17 +984,70 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list">
+      <formula1>"geturl,find element"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="13.5703125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="18.7109375" collapsed="true"/>
@@ -958,13 +1090,13 @@
         <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1038,6 +1170,34 @@
       </c>
       <c r="D8" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1053,10 +1213,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B8" type="list">
+    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B10" type="list">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C8" type="list">
+    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C10" type="list">
       <formula1>"FireFox,Chrome,Internet Explorer,Phantom JS"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1069,7 +1229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1126,19 +1286,19 @@
     </row>
     <row r="3" spans="1:9">
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
         <v>51</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1146,7 +1306,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1488,7 +1648,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1499,13 +1659,13 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1537,10 +1697,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1573,10 +1733,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1591,17 +1751,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G3"/>
+  <dimension ref="A2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="11.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="42.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="45.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7">
@@ -1609,7 +1769,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1617,12 +1777,39 @@
     </row>
     <row r="3" spans="3:7">
       <c r="C3" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1634,4 +1821,89 @@
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list">
+      <formula1>"geturl,find element"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
object repository dynamic x path handling,support date picker
</commit_message>
<xml_diff>
--- a/mavenHybrid/webdriver/excelLib.xlsx
+++ b/mavenHybrid/webdriver/excelLib.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="9" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="4050"/>
+    <workbookView activeTab="1" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="4050"/>
   </bookViews>
   <sheets>
     <sheet name="login" r:id="rId1" sheetId="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="65">
   <si>
     <t>SpecialActionType</t>
   </si>
@@ -211,40 +211,13 @@
     <t>seleniumupload</t>
   </si>
   <si>
-    <t>FAIL unknown error: path is not absolute: file:///c:/users/partha/desktop/uploadfile.html
-  (Session info: chrome=56.0.2924.87)
-  (Driver info: chromedriver=2.28.455520 (cc17746adff54984afff480136733114c6b3704b),platform=Windows NT 6.3.9600 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 75 milliseconds
-Build info: version: 'unknown', revision: 'b526bd5', time: '2017-03-07 11:11:07 -0800'
-System info: host: 'SAI', ip: '127.0.0.1', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '1.8.0_121'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.28.455520 (cc17746adff54984afff480136733114c6b3704b), userDataDir=C:\Users\partha\AppData\Local\Temp\scoped_dir6436_12744}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=WIN8_1, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=accept}]
-Session ID: 5226fb890b8e5d324e74d64b9c653781</t>
-  </si>
-  <si>
-    <t>/log4j.properties</t>
-  </si>
-  <si>
-    <t>FAIL unknown error: path is not absolute: /log4j.properties
-  (Session info: chrome=56.0.2924.87)
-  (Driver info: chromedriver=2.28.455520 (cc17746adff54984afff480136733114c6b3704b),platform=Windows NT 6.3.9600 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 78 milliseconds
-Build info: version: 'unknown', revision: 'b526bd5', time: '2017-03-07 11:11:07 -0800'
-System info: host: 'SAI', ip: '127.0.0.1', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '1.8.0_121'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.28.455520 (cc17746adff54984afff480136733114c6b3704b), userDataDir=C:\Users\partha\AppData\Local\Temp\scoped_dir5260_12812}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=WIN8_1, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=accept}]
-Session ID: 4bd76188c6e65184753f8e2a304a92e0</t>
-  </si>
-  <si>
-    <t>FAIL unknown error: path is not absolute: /log4j.properties
-  (Session info: chrome=56.0.2924.87)
-  (Driver info: chromedriver=2.28.455520 (cc17746adff54984afff480136733114c6b3704b),platform=Windows NT 6.3.9600 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 78 milliseconds
-Build info: version: 'unknown', revision: 'b526bd5', time: '2017-03-07 11:11:07 -0800'
-System info: host: 'SAI', ip: '127.0.0.1', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '1.8.0_121'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.28.455520 (cc17746adff54984afff480136733114c6b3704b), userDataDir=C:\Users\partha\AppData\Local\Temp\scoped_dir6928_1117}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=WIN8_1, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=accept}]
-Session ID: ed86483c450b6d3ac31d332b40c59007</t>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>FAIL null</t>
+  </si>
+  <si>
+    <t>FAIL Expected condition failed: waiting for hybridFramework.webdriver.MultiGetelement$1@4e31c3ec (tried for 60 second(s) with 250 MILLISECONDS interval)</t>
   </si>
 </sst>
 </file>
@@ -252,19 +225,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -339,26 +305,23 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
@@ -369,7 +332,45 @@
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -809,7 +810,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -959,18 +960,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J1">
-    <cfRule dxfId="18" priority="1" stopIfTrue="1" type="expression">
+    <cfRule dxfId="22" priority="1" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
     </cfRule>
-    <cfRule dxfId="17" priority="2" stopIfTrue="1" type="expression">
+    <cfRule dxfId="21" priority="2" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule dxfId="16" priority="3" stopIfTrue="1" type="expression">
+    <cfRule dxfId="20" priority="3" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",H1)))</formula>
     </cfRule>
-    <cfRule dxfId="15" priority="4" stopIfTrue="1" type="expression">
+    <cfRule dxfId="19" priority="4" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -986,50 +987,171 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G3"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7">
+    <row r="1" spans="1:10">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="3:7">
+    <row r="3" spans="1:10">
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
         <v>63</v>
       </c>
-      <c r="G3" t="s">
-        <v>65</v>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I1:J1">
+    <cfRule dxfId="3" priority="1" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
+    </cfRule>
+    <cfRule dxfId="2" priority="2" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule dxfId="1" priority="3" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("fail",H1)))</formula>
+    </cfRule>
+    <cfRule dxfId="0" priority="4" stopIfTrue="1" type="expression">
+      <formula>NOT(ISERROR(SEARCH("pass",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C8" type="list">
       <formula1>"geturl,find element"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1041,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1202,13 +1324,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule dxfId="14" operator="equal" priority="3" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="18" operator="equal" priority="3" stopIfTrue="1" type="cellIs">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="13" operator="equal" priority="4" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="17" operator="equal" priority="4" stopIfTrue="1" type="cellIs">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule dxfId="12" operator="equal" priority="5" stopIfTrue="1" type="cellIs">
+    <cfRule dxfId="16" operator="equal" priority="5" stopIfTrue="1" type="cellIs">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1311,26 +1433,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1">
-    <cfRule dxfId="11" priority="3" stopIfTrue="1" type="expression">
+    <cfRule dxfId="15" priority="3" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
     </cfRule>
-    <cfRule dxfId="10" priority="4" stopIfTrue="1" type="expression">
+    <cfRule dxfId="14" priority="4" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule dxfId="9" priority="5" stopIfTrue="1" type="expression">
+    <cfRule dxfId="13" priority="5" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",H1)))</formula>
     </cfRule>
-    <cfRule dxfId="8" priority="6" stopIfTrue="1" type="expression">
+    <cfRule dxfId="12" priority="6" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule dxfId="7" operator="containsText" priority="1" text="fail" type="containsText">
+    <cfRule dxfId="11" operator="containsText" priority="1" text="fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("fail",G1)))</formula>
     </cfRule>
-    <cfRule dxfId="6" operator="containsText" priority="2" text="pass" type="containsText">
+    <cfRule dxfId="10" operator="containsText" priority="2" text="pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("pass",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1538,26 +1660,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1">
-    <cfRule dxfId="5" priority="3" stopIfTrue="1" type="expression">
+    <cfRule dxfId="9" priority="3" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",I1)))</formula>
     </cfRule>
-    <cfRule dxfId="4" priority="4" stopIfTrue="1" type="expression">
+    <cfRule dxfId="8" priority="4" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule dxfId="3" priority="5" stopIfTrue="1" type="expression">
+    <cfRule dxfId="7" priority="5" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("fail",H1)))</formula>
     </cfRule>
-    <cfRule dxfId="2" priority="6" stopIfTrue="1" type="expression">
+    <cfRule dxfId="6" priority="6" stopIfTrue="1" type="expression">
       <formula>NOT(ISERROR(SEARCH("pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G3">
-    <cfRule dxfId="1" operator="containsText" priority="1" text="fail" type="containsText">
+    <cfRule dxfId="5" operator="containsText" priority="1" text="fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("fail",G1)))</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="containsText" priority="2" text="pass" type="containsText">
+    <cfRule dxfId="4" operator="containsText" priority="2" text="pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("pass",G1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Check all links performance tuning,File upload
</commit_message>
<xml_diff>
--- a/mavenHybrid/webdriver/excelLib.xlsx
+++ b/mavenHybrid/webdriver/excelLib.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6390" windowWidth="14910" xWindow="5145" yWindow="4050"/>
+    <workbookView activeTab="9" firstSheet="1" windowHeight="6390" windowWidth="19620" xWindow="435" yWindow="1650"/>
   </bookViews>
   <sheets>
     <sheet name="login" r:id="rId1" sheetId="1"/>
@@ -17,13 +17,14 @@
     <sheet name="sikuli" r:id="rId8" sheetId="8"/>
     <sheet name="sikuliselenium" r:id="rId9" sheetId="9"/>
     <sheet name="seleniumupload" r:id="rId10" sheetId="10"/>
+    <sheet name="robotupload" r:id="rId11" sheetId="11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="66">
   <si>
     <t>SpecialActionType</t>
   </si>
@@ -211,13 +212,16 @@
     <t>seleniumupload</t>
   </si>
   <si>
-    <t>clear</t>
-  </si>
-  <si>
-    <t>FAIL null</t>
-  </si>
-  <si>
-    <t>FAIL Expected condition failed: waiting for hybridFramework.webdriver.MultiGetelement$1@4e31c3ec (tried for 60 second(s) with 250 MILLISECONDS interval)</t>
+    <t>robotupload</t>
+  </si>
+  <si>
+    <t>checkallimages</t>
+  </si>
+  <si>
+    <t>checkalllinks</t>
+  </si>
+  <si>
+    <t>https://www.html5rocks.com/en/</t>
   </si>
 </sst>
 </file>
@@ -225,12 +229,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -305,23 +316,26 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
@@ -987,15 +1001,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
@@ -1037,7 +1051,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1045,13 +1059,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -1059,77 +1067,9 @@
     </row>
     <row r="4" spans="1:10">
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1151,7 +1091,95 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C8" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2" type="list">
+      <formula1>"geturl,find element"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="2.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list">
       <formula1>"geturl,find element"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1161,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1322,6 +1350,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule dxfId="18" operator="equal" priority="3" stopIfTrue="1" type="cellIs">
@@ -1335,10 +1377,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B10" type="list">
+    <dataValidation allowBlank="1" prompt="Should add to suite?" promptTitle="STATUS" showErrorMessage="1" showInputMessage="1" sqref="B2:B11" type="list">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C10" type="list">
+    <dataValidation allowBlank="1" prompt="Please select broser type" showErrorMessage="1" showInputMessage="1" sqref="C2:C11" type="list">
       <formula1>"FireFox,Chrome,Internet Explorer,Phantom JS"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>